<commit_message>
Actor System spport for Topic
</commit_message>
<xml_diff>
--- a/Results/Performance/Performance results paper 1.xlsx
+++ b/Results/Performance/Performance results paper 1.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\NeoCortex\Results\Performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7925679-165E-4CD0-8973-CE886FA09D8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF2BAAB-21E0-4ECB-9720-DBECBEBF6390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{DBA58A64-707E-4E76-BD3F-46D9BD9F43F7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" firstSheet="1" activeTab="1" xr2:uid="{DBA58A64-707E-4E76-BD3F-46D9BD9F43F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SPMT vs. SP COmpute performance" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="SPMT - topology performance" sheetId="4" r:id="rId2"/>
+    <sheet name="SPParallel" sheetId="2" r:id="rId3"/>
+    <sheet name="SPMT - Memory consumption" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A:$A</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B:$B</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'SPMT vs. SP COmpute performance'!$A:$A</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'SPMT vs. SP COmpute performance'!$B:$B</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,12 +38,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t xml:space="preserve">Init time SP </t>
   </si>
   <si>
     <t>Init Time SPMT</t>
+  </si>
+  <si>
+    <t>Compute Time: 28x28, Cols 200x200 3 Nodes</t>
+  </si>
+  <si>
+    <t>approx. 20 min</t>
+  </si>
+  <si>
+    <t>Compute Time: 28x28, Cols 200x200  2 Nodes</t>
+  </si>
+  <si>
+    <t>approx. 55 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spatial Pooler MT : Cols=64x64 in MB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spatial Pooler MT : Cols=32x32 in MB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spatial Pooler MT : Cols=128x128 in MB </t>
+  </si>
+  <si>
+    <t>28x28, Cols=32*32</t>
+  </si>
+  <si>
+    <t>64x64</t>
+  </si>
+  <si>
+    <t>30 per min</t>
+  </si>
+  <si>
+    <t>Inp:28x28, Cols 64x64 in sec</t>
+  </si>
+  <si>
+    <t>Inp:28x28, Cols 128x128 in sec</t>
+  </si>
+  <si>
+    <t>6 per min</t>
+  </si>
+  <si>
+    <t>Inp:28x28, Cols 200x200 in sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spatial Pooler MT : Cols=200x200 in MB </t>
+  </si>
+  <si>
+    <t>Inp:28x28, Cols 32x32 in sec</t>
+  </si>
+  <si>
+    <t>12-15 per min</t>
+  </si>
+  <si>
+    <t>32x32</t>
+  </si>
+  <si>
+    <t>128x128</t>
+  </si>
+  <si>
+    <t>200x200</t>
   </si>
 </sst>
 </file>
@@ -56,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -76,8 +145,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -93,6 +164,593 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Compute time in ms]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SPMT - topology performance'!$D$1:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32x32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64x64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128x128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200x200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SPMT - topology performance'!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3600-4CDA-B0C5-FF0EDD8D8E46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="423021744"/>
+        <c:axId val="423029616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="423021744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423029616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="423029616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423021744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Occupied memory </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SPMT - Memory consumption'!$D$2:$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32x32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64x64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128x128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200x200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SPMT - Memory consumption'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-77EE-42D5-89C4-002198EBE7D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="571895984"/>
+        <c:axId val="332879648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="571895984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="332879648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="332879648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="571895984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -271,6 +929,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
@@ -1297,6 +2035,1038 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1462,6 +3232,88 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7EF7B7C-A55B-45D1-BC85-D0318046A0D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>895349</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F082277-7F97-4004-922D-BE20B58822BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1761,8 +3613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2B9CF5-6F4E-4B5F-80C9-17B5C01F427E}">
   <dimension ref="A1:K260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="O63" sqref="O63"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2286,6 +4138,9 @@
       <c r="B63">
         <v>65</v>
       </c>
+      <c r="G63" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64">
@@ -3459,6 +5314,224 @@
     <row r="260" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B260">
         <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D92001-D2AD-417A-A22F-08E3D4A55928}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="25.9296875" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1">
+        <v>200</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>2000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>5000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4545209-8F0A-46A9-8C83-B8551A47A546}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="55.19921875" customWidth="1"/>
+    <col min="2" max="2" width="49.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1329640</v>
+      </c>
+      <c r="B2">
+        <v>3240000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1352106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1298728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>1305753</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>1345149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>1294736</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E449699B-FFF6-41DB-AE6E-253FE1AB9413}">
+  <dimension ref="B1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>165</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>600</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>2200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>5400</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added unittest for perfromance data parsing
</commit_message>
<xml_diff>
--- a/Results/Performance/Performance results paper 1.xlsx
+++ b/Results/Performance/Performance results paper 1.xlsx
@@ -8,19 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\NeoCortex\Results\Performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF2BAAB-21E0-4ECB-9720-DBECBEBF6390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3368183F-E4DC-4DE9-8872-594C5B4DE743}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" firstSheet="1" activeTab="1" xr2:uid="{DBA58A64-707E-4E76-BD3F-46D9BD9F43F7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" firstSheet="1" activeTab="2" xr2:uid="{DBA58A64-707E-4E76-BD3F-46D9BD9F43F7}"/>
   </bookViews>
   <sheets>
     <sheet name="SPMT vs. SP COmpute performance" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="SPMT - topology performance" sheetId="4" r:id="rId2"/>
     <sheet name="SPParallel" sheetId="2" r:id="rId3"/>
-    <sheet name="SPMT - Memory consumption" sheetId="3" r:id="rId4"/>
+    <sheet name="Init time" sheetId="5" r:id="rId4"/>
+    <sheet name="SPMT - Memory consumption" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'SPMT vs. SP COmpute performance'!$A:$A</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'SPMT vs. SP COmpute performance'!$B:$B</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">SPParallel!$A$12:$A$39</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">SPParallel!$A$12:$A$496</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">SPParallel!$B$12:$B$28</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">SPParallel!$B$12:$B$57</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">SPParallel!$C$12:$C$152</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">SPParallel!$C$12:$C$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,15 +45,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t xml:space="preserve">Init time SP </t>
   </si>
   <si>
     <t>Init Time SPMT</t>
-  </si>
-  <si>
-    <t>Compute Time: 28x28, Cols 200x200 3 Nodes</t>
   </si>
   <si>
     <t>approx. 20 min</t>
@@ -104,6 +108,33 @@
   </si>
   <si>
     <t>200x200</t>
+  </si>
+  <si>
+    <t>Compute Time: 28x28, Cols 200x200 3 Nodes with persistence</t>
+  </si>
+  <si>
+    <t>Compute Time: 28x28, Cols 200x200 3 Nodes without persistence 15 partitions</t>
+  </si>
+  <si>
+    <t>Compute Time: 28x28, Cols 200x200 2 Nodes without persistence, 20 partitions</t>
+  </si>
+  <si>
+    <t>Single node. Running locally</t>
+  </si>
+  <si>
+    <t>RAM on local box SP-MT algorithm</t>
+  </si>
+  <si>
+    <t>Compute Time: 28x28, Cols 200x200 1 Node without persistence 15 partitions</t>
+  </si>
+  <si>
+    <t>3 nodes</t>
+  </si>
+  <si>
+    <t>2 nodes</t>
+  </si>
+  <si>
+    <t>1 node</t>
   </si>
 </sst>
 </file>
@@ -181,6 +212,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Compute time in ms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -569,7 +625,7 @@
                   <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5400</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,6 +905,76 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.6</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000000-129A-4340-86FF-716A018A30FC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>3 nodes</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-129A-4340-86FF-716A018A30FC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>2 nodes</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000002-129A-4340-86FF-716A018A30FC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>1 Node</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1009,6 +1135,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
@@ -2556,6 +2722,521 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3274,6 +3955,89 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0372E21B-4627-4FBC-A0B7-37AAC18B40BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15335249" y="12363450"/>
+              <a:ext cx="5657850" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4139,7 +4903,7 @@
         <v>65</v>
       </c>
       <c r="G63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
@@ -5326,8 +6090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D92001-D2AD-417A-A22F-08E3D4A55928}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5338,55 +6102,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1">
         <v>200</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>2000</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>5000</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>10000</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5397,27 +6161,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4545209-8F0A-46A9-8C83-B8551A47A546}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C496"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="55.19921875" customWidth="1"/>
-    <col min="2" max="2" width="49.06640625" customWidth="1"/>
+    <col min="2" max="2" width="64.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1329640</v>
       </c>
@@ -5425,37 +6190,3077 @@
         <v>3240000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1352106</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1298728</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1305753</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1345149</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1294736</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>17627</v>
+      </c>
+      <c r="B12">
+        <v>1396</v>
+      </c>
+      <c r="C12">
+        <v>6451</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>19634</v>
+      </c>
+      <c r="B13">
+        <v>2451</v>
+      </c>
+      <c r="C13">
+        <v>6265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>5032</v>
+      </c>
+      <c r="B14">
+        <v>5812</v>
+      </c>
+      <c r="C14">
+        <v>6831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>4756</v>
+      </c>
+      <c r="B15">
+        <v>6003</v>
+      </c>
+      <c r="C15">
+        <v>6094</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>4808</v>
+      </c>
+      <c r="B16">
+        <v>8469</v>
+      </c>
+      <c r="C16">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>3291</v>
+      </c>
+      <c r="B17">
+        <v>4178</v>
+      </c>
+      <c r="C17">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>3181</v>
+      </c>
+      <c r="B18">
+        <v>4037</v>
+      </c>
+      <c r="C18">
+        <v>4353</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>3229</v>
+      </c>
+      <c r="B19">
+        <v>3677</v>
+      </c>
+      <c r="C19">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>3505</v>
+      </c>
+      <c r="B20">
+        <v>3786</v>
+      </c>
+      <c r="C20">
+        <v>4146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>3448</v>
+      </c>
+      <c r="B21">
+        <v>3732</v>
+      </c>
+      <c r="C21">
+        <v>6975</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>3260</v>
+      </c>
+      <c r="B22">
+        <v>3914</v>
+      </c>
+      <c r="C22">
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>3472</v>
+      </c>
+      <c r="B23">
+        <v>4041</v>
+      </c>
+      <c r="C23">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>3342</v>
+      </c>
+      <c r="B24">
+        <v>4672</v>
+      </c>
+      <c r="C24">
+        <v>4135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>4113</v>
+      </c>
+      <c r="B25">
+        <v>5670</v>
+      </c>
+      <c r="C25">
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>3310</v>
+      </c>
+      <c r="B26">
+        <v>4866</v>
+      </c>
+      <c r="C26">
+        <v>4664</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>8099</v>
+      </c>
+      <c r="B27">
+        <v>8801</v>
+      </c>
+      <c r="C27">
+        <v>21137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>6233</v>
+      </c>
+      <c r="B28">
+        <v>7303</v>
+      </c>
+      <c r="C28">
+        <v>10770</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>5309</v>
+      </c>
+      <c r="B29">
+        <v>2426</v>
+      </c>
+      <c r="C29">
+        <v>6064</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>4657</v>
+      </c>
+      <c r="B30">
+        <v>1031</v>
+      </c>
+      <c r="C30">
+        <v>5926</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>4961</v>
+      </c>
+      <c r="B31">
+        <v>6709</v>
+      </c>
+      <c r="C31">
+        <v>6033</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>4449</v>
+      </c>
+      <c r="B32">
+        <v>1011</v>
+      </c>
+      <c r="C32">
+        <v>6808</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>4787</v>
+      </c>
+      <c r="B33">
+        <v>9103</v>
+      </c>
+      <c r="C33">
+        <v>5880</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>4738</v>
+      </c>
+      <c r="B34">
+        <v>6528</v>
+      </c>
+      <c r="C34">
+        <v>8558</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>4484</v>
+      </c>
+      <c r="B35">
+        <v>6284</v>
+      </c>
+      <c r="C35">
+        <v>17802</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>5045</v>
+      </c>
+      <c r="B36">
+        <v>6238</v>
+      </c>
+      <c r="C36">
+        <v>7474</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>4789</v>
+      </c>
+      <c r="B37">
+        <v>9305</v>
+      </c>
+      <c r="C37">
+        <v>6164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>4886</v>
+      </c>
+      <c r="B38">
+        <v>5913</v>
+      </c>
+      <c r="C38">
+        <v>7444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>4830</v>
+      </c>
+      <c r="B39">
+        <v>9026</v>
+      </c>
+      <c r="C39">
+        <v>12589</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>4623</v>
+      </c>
+      <c r="B40">
+        <v>6004</v>
+      </c>
+      <c r="C40">
+        <v>5661</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>5072</v>
+      </c>
+      <c r="B41">
+        <v>8404</v>
+      </c>
+      <c r="C41">
+        <v>5972</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>5877</v>
+      </c>
+      <c r="B42">
+        <v>6057</v>
+      </c>
+      <c r="C42">
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>4649</v>
+      </c>
+      <c r="B43">
+        <v>5506</v>
+      </c>
+      <c r="C43">
+        <v>5985</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>5154</v>
+      </c>
+      <c r="B44">
+        <v>5898</v>
+      </c>
+      <c r="C44">
+        <v>6008</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>4754</v>
+      </c>
+      <c r="B45">
+        <v>6305</v>
+      </c>
+      <c r="C45">
+        <v>5910</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>4340</v>
+      </c>
+      <c r="B46">
+        <v>6404</v>
+      </c>
+      <c r="C46">
+        <v>6086</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>4877</v>
+      </c>
+      <c r="B47">
+        <v>7001</v>
+      </c>
+      <c r="C47">
+        <v>5745</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>5683</v>
+      </c>
+      <c r="B48">
+        <v>6160</v>
+      </c>
+      <c r="C48">
+        <v>7164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>4594</v>
+      </c>
+      <c r="B49">
+        <v>6412</v>
+      </c>
+      <c r="C49">
+        <v>5983</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>4720</v>
+      </c>
+      <c r="B50">
+        <v>6119</v>
+      </c>
+      <c r="C50">
+        <v>6048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>4583</v>
+      </c>
+      <c r="B51">
+        <v>6611</v>
+      </c>
+      <c r="C51">
+        <v>5465</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>3395</v>
+      </c>
+      <c r="B52">
+        <v>5192</v>
+      </c>
+      <c r="C52">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>5341</v>
+      </c>
+      <c r="B53">
+        <v>3995</v>
+      </c>
+      <c r="C53">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>3812</v>
+      </c>
+      <c r="B54">
+        <v>4242</v>
+      </c>
+      <c r="C54">
+        <v>4142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>5040</v>
+      </c>
+      <c r="B55">
+        <v>4478</v>
+      </c>
+      <c r="C55">
+        <v>4409</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>3431</v>
+      </c>
+      <c r="B56">
+        <v>4402</v>
+      </c>
+      <c r="C56">
+        <v>4289</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>3612</v>
+      </c>
+      <c r="B57">
+        <v>4045</v>
+      </c>
+      <c r="C57">
+        <v>4354</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>3511</v>
+      </c>
+      <c r="C58">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>3750</v>
+      </c>
+      <c r="C59">
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>4239</v>
+      </c>
+      <c r="C60">
+        <v>4715</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>3097</v>
+      </c>
+      <c r="C61">
+        <v>4734</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>20976</v>
+      </c>
+      <c r="C62">
+        <v>66136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>20643</v>
+      </c>
+      <c r="C63">
+        <v>63113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>15975</v>
+      </c>
+      <c r="C64">
+        <v>51958</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>10156</v>
+      </c>
+      <c r="C65">
+        <v>19560</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>7078</v>
+      </c>
+      <c r="C66">
+        <v>8480</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>5266</v>
+      </c>
+      <c r="C67">
+        <v>5476</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>5127</v>
+      </c>
+      <c r="C68">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>4636</v>
+      </c>
+      <c r="C69">
+        <v>5516</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>4352</v>
+      </c>
+      <c r="C70">
+        <v>7202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>4904</v>
+      </c>
+      <c r="C71">
+        <v>5178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>5675</v>
+      </c>
+      <c r="C72">
+        <v>3925</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>3964</v>
+      </c>
+      <c r="C73">
+        <v>4163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>3742</v>
+      </c>
+      <c r="C74">
+        <v>4298</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>3091</v>
+      </c>
+      <c r="C75">
+        <v>4245</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>3355</v>
+      </c>
+      <c r="C76">
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>3521</v>
+      </c>
+      <c r="C77">
+        <v>4313</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>3306</v>
+      </c>
+      <c r="C78">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>3726</v>
+      </c>
+      <c r="C79">
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>3640</v>
+      </c>
+      <c r="C80">
+        <v>4373</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>3412</v>
+      </c>
+      <c r="C81">
+        <v>4162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>18389</v>
+      </c>
+      <c r="C82">
+        <v>13546</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>4739</v>
+      </c>
+      <c r="C83">
+        <v>6016</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>6103</v>
+      </c>
+      <c r="C84">
+        <v>5161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>4167</v>
+      </c>
+      <c r="C85">
+        <v>5723</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>4288</v>
+      </c>
+      <c r="C86">
+        <v>5312</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>5390</v>
+      </c>
+      <c r="C87">
+        <v>19661</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>14859</v>
+      </c>
+      <c r="C88">
+        <v>8506</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>4505</v>
+      </c>
+      <c r="C89">
+        <v>6124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>4257</v>
+      </c>
+      <c r="C90">
+        <v>5125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>4335</v>
+      </c>
+      <c r="C91">
+        <v>5476</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>5586</v>
+      </c>
+      <c r="C92">
+        <v>5719</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>4316</v>
+      </c>
+      <c r="C93">
+        <v>5816</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>4446</v>
+      </c>
+      <c r="C94">
+        <v>5719</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>4178</v>
+      </c>
+      <c r="C95">
+        <v>4996</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>3927</v>
+      </c>
+      <c r="C96">
+        <v>4980</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>3346</v>
+      </c>
+      <c r="C97">
+        <v>5207</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>3384</v>
+      </c>
+      <c r="C98">
+        <v>4233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>3722</v>
+      </c>
+      <c r="C99">
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>3453</v>
+      </c>
+      <c r="C100">
+        <v>4730</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>3071</v>
+      </c>
+      <c r="C101">
+        <v>5783</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>14408</v>
+      </c>
+      <c r="C102">
+        <v>21103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>15017</v>
+      </c>
+      <c r="C103">
+        <v>18842</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>4598</v>
+      </c>
+      <c r="C104">
+        <v>5524</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>4770</v>
+      </c>
+      <c r="C105">
+        <v>5152</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>4072</v>
+      </c>
+      <c r="C106">
+        <v>5696</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>6360</v>
+      </c>
+      <c r="C107">
+        <v>7686</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>4802</v>
+      </c>
+      <c r="C108">
+        <v>6042</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>6427</v>
+      </c>
+      <c r="C109">
+        <v>5534</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>9372</v>
+      </c>
+      <c r="C110">
+        <v>6349</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>10342</v>
+      </c>
+      <c r="C111">
+        <v>5501</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>8699</v>
+      </c>
+      <c r="C112">
+        <v>6265</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>8951</v>
+      </c>
+      <c r="C113">
+        <v>5884</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>9719</v>
+      </c>
+      <c r="C114">
+        <v>5547</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>5207</v>
+      </c>
+      <c r="C115">
+        <v>5431</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>3768</v>
+      </c>
+      <c r="C116">
+        <v>5095</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>5194</v>
+      </c>
+      <c r="C117">
+        <v>6073</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>6699</v>
+      </c>
+      <c r="C118">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>4144</v>
+      </c>
+      <c r="C119">
+        <v>5386</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>4623</v>
+      </c>
+      <c r="C120">
+        <v>4943</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>3936</v>
+      </c>
+      <c r="C121">
+        <v>5248</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A122">
+        <v>8728</v>
+      </c>
+      <c r="C122">
+        <v>5807</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A123">
+        <v>5013</v>
+      </c>
+      <c r="C123">
+        <v>5559</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A124">
+        <v>5007</v>
+      </c>
+      <c r="C124">
+        <v>5819</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A125">
+        <v>4937</v>
+      </c>
+      <c r="C125">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A126">
+        <v>5134</v>
+      </c>
+      <c r="C126">
+        <v>5807</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A127">
+        <v>4996</v>
+      </c>
+      <c r="C127">
+        <v>6005</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A128">
+        <v>4901</v>
+      </c>
+      <c r="C128">
+        <v>6024</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A129">
+        <v>4788</v>
+      </c>
+      <c r="C129">
+        <v>5341</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A130">
+        <v>4013</v>
+      </c>
+      <c r="C130">
+        <v>4685</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A131">
+        <v>4524</v>
+      </c>
+      <c r="C131">
+        <v>5453</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A132">
+        <v>4918</v>
+      </c>
+      <c r="C132">
+        <v>6152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A133">
+        <v>5191</v>
+      </c>
+      <c r="C133">
+        <v>5258</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A134">
+        <v>4161</v>
+      </c>
+      <c r="C134">
+        <v>5052</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A135">
+        <v>3954</v>
+      </c>
+      <c r="C135">
+        <v>7371</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A136">
+        <v>3714</v>
+      </c>
+      <c r="C136">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A137">
+        <v>3604</v>
+      </c>
+      <c r="C137">
+        <v>4188</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A138">
+        <v>3074</v>
+      </c>
+      <c r="C138">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A139">
+        <v>3184</v>
+      </c>
+      <c r="C139">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A140">
+        <v>3566</v>
+      </c>
+      <c r="C140">
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A141">
+        <v>3661</v>
+      </c>
+      <c r="C141">
+        <v>4876</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A142">
+        <v>12636</v>
+      </c>
+      <c r="C142">
+        <v>6497</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A143">
+        <v>13219</v>
+      </c>
+      <c r="C143">
+        <v>6564</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A144">
+        <v>4336</v>
+      </c>
+      <c r="C144">
+        <v>5076</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A145">
+        <v>4109</v>
+      </c>
+      <c r="C145">
+        <v>4830</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A146">
+        <v>3865</v>
+      </c>
+      <c r="C146">
+        <v>5493</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A147">
+        <v>6506</v>
+      </c>
+      <c r="C147">
+        <v>6057</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A148">
+        <v>5026</v>
+      </c>
+      <c r="C148">
+        <v>6761</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A149">
+        <v>4563</v>
+      </c>
+      <c r="C149">
+        <v>7677</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A150">
+        <v>4100</v>
+      </c>
+      <c r="C150">
+        <v>9475</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A151">
+        <v>3706</v>
+      </c>
+      <c r="C151">
+        <v>5492</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A152">
+        <v>4904</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A153">
+        <v>5086</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A154">
+        <v>4149</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A155">
+        <v>4199</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A156">
+        <v>4337</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A157">
+        <v>3823</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A158">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A159">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A160">
+        <v>3481</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A161">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A162">
+        <v>5189</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A163">
+        <v>5507</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A164">
+        <v>4622</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A165">
+        <v>5799</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A166">
+        <v>9686</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A167">
+        <v>5378</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A168">
+        <v>9902</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A169">
+        <v>4870</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A170">
+        <v>6192</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A171">
+        <v>4142</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A172">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A173">
+        <v>3902</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A174">
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A175">
+        <v>7618</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A176">
+        <v>3897</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A177">
+        <v>14525</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A178">
+        <v>13303</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A179">
+        <v>4893</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A180">
+        <v>4884</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A181">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A182">
+        <v>5303</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A183">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A184">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A185">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A186">
+        <v>4044</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A187">
+        <v>5281</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A188">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A189">
+        <v>4336</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A190">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A191">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A192">
+        <v>4708</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A193">
+        <v>4971</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A194">
+        <v>4652</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A195">
+        <v>4511</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A196">
+        <v>4493</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A197">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A198">
+        <v>4705</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A199">
+        <v>5211</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A200">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A201">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A202">
+        <v>5669</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A203">
+        <v>4933</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A204">
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A205">
+        <v>4139</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A206">
+        <v>3895</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A207">
+        <v>4957</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A208">
+        <v>4505</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A209">
+        <v>4710</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A210">
+        <v>5127</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A211">
+        <v>5150</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A212">
+        <v>5031</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A213">
+        <v>4955</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A214">
+        <v>5257</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A215">
+        <v>4647</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A216">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A217">
+        <v>5279</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A218">
+        <v>4921</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A219">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A220">
+        <v>4496</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A221">
+        <v>6883</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A222">
+        <v>6222</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A223">
+        <v>4051</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A224">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A225">
+        <v>5706</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A226">
+        <v>5057</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A227">
+        <v>29924</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A228">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A229">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A230">
+        <v>4069</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A231">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A232">
+        <v>4671</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A233">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A234">
+        <v>4443</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A235">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A236">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A237">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A238">
+        <v>5070</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A239">
+        <v>6259</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A240">
+        <v>5476</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A241">
+        <v>4978</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A242">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A243">
+        <v>4549</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A244">
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A245">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A246">
+        <v>3645</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A247">
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A248">
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A249">
+        <v>3228</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A250">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A251">
+        <v>3411</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A252">
+        <v>20113</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A253">
+        <v>4318</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A254">
+        <v>4525</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A255">
+        <v>5021</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A256">
+        <v>3646</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A257">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A258">
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A259">
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A260">
+        <v>4076</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A261">
+        <v>3884</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A262">
+        <v>10636</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A263">
+        <v>5118</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A264">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A265">
+        <v>4387</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A266">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A267">
+        <v>4821</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A268">
+        <v>4882</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A269">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A270">
+        <v>4206</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A271">
+        <v>5295</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A272">
+        <v>5460</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A273">
+        <v>4732</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A274">
+        <v>4976</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A275">
+        <v>4892</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A276">
+        <v>5851</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A277">
+        <v>9141</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A278">
+        <v>5006</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A279">
+        <v>6053</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A280">
+        <v>6866</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A281">
+        <v>9024</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A282">
+        <v>16609</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A283">
+        <v>5430</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A284">
+        <v>10447</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A285">
+        <v>5344</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A286">
+        <v>5213</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A287">
+        <v>6752</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A288">
+        <v>4689</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A289">
+        <v>4427</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A290">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A291">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A292">
+        <v>5836</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A293">
+        <v>5086</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A294">
+        <v>4605</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A295">
+        <v>4082</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A296">
+        <v>3965</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A297">
+        <v>3434</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A298">
+        <v>3412</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A299">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A300">
+        <v>3598</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A301">
+        <v>3413</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A302">
+        <v>13282</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A303">
+        <v>13462</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A304">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A305">
+        <v>4934</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A306">
+        <v>5271</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A307">
+        <v>5621</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A308">
+        <v>6090</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A309">
+        <v>9220</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A310">
+        <v>5166</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A311">
+        <v>5093</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A312">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A313">
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A314">
+        <v>4834</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A315">
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A316">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A317">
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A318">
+        <v>4959</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A319">
+        <v>4626</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A320">
+        <v>4978</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A321">
+        <v>5137</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A322">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A323">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A324">
+        <v>3391</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A325">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A326">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A327">
+        <v>4931</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A328">
+        <v>4665</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A329">
+        <v>5398</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A330">
+        <v>8859</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A331">
+        <v>6440</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A332">
+        <v>9407</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A333">
+        <v>8063</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A334">
+        <v>5322</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A335">
+        <v>5064</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A336">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A337">
+        <v>3862</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A338">
+        <v>3462</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A339">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A340">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A341">
+        <v>3414</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A342">
+        <v>5059</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A343">
+        <v>12195</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A344">
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A345">
+        <v>5392</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A346">
+        <v>6848</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A347">
+        <v>4774</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A348">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A349">
+        <v>6727</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A350">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A351">
+        <v>4931</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A352">
+        <v>5403</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A353">
+        <v>5207</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A354">
+        <v>5229</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A355">
+        <v>4796</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A356">
+        <v>4515</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A357">
+        <v>5349</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A358">
+        <v>5930</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A359">
+        <v>5063</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A360">
+        <v>5399</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A361">
+        <v>6056</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A362">
+        <v>4177</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A363">
+        <v>3573</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A364">
+        <v>3613</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A365">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A366">
+        <v>3543</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A367">
+        <v>15517</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A368">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A369">
+        <v>4991</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A370">
+        <v>5275</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A371">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A372">
+        <v>4709</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A373">
+        <v>5499</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A374">
+        <v>4854</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A375">
+        <v>5168</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A376">
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A377">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A378">
+        <v>3689</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A379">
+        <v>3297</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A380">
+        <v>3976</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A381">
+        <v>3402</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A382">
+        <v>3779</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A383">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A384">
+        <v>4451</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A385">
+        <v>6914</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A386">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A387">
+        <v>3676</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A388">
+        <v>5446</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A389">
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A390">
+        <v>5382</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A391">
+        <v>7620</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A392">
+        <v>3511</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A393">
+        <v>4386</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A394">
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A395">
+        <v>3539</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A396">
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A397">
+        <v>3332</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A398">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A399">
+        <v>3692</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A400">
+        <v>4716</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A401">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A402">
+        <v>20150</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A403">
+        <v>10099</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A404">
+        <v>16149</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A405">
+        <v>5551</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A406">
+        <v>5239</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A407">
+        <v>11571</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A408">
+        <v>5229</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A409">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A410">
+        <v>4102</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A411">
+        <v>3913</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A412">
+        <v>6938</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A413">
+        <v>4546</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A414">
+        <v>4723</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A415">
+        <v>5014</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A416">
+        <v>5693</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A417">
+        <v>5129</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A418">
+        <v>4840</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A419">
+        <v>4660</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A420">
+        <v>4237</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A421">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A422">
+        <v>5204</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A423">
+        <v>5117</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A424">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A425">
+        <v>4397</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A426">
+        <v>4710</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A427">
+        <v>4791</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A428">
+        <v>5356</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A429">
+        <v>5525</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A430">
+        <v>5707</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A431">
+        <v>5155</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A432">
+        <v>5516</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A433">
+        <v>5406</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A434">
+        <v>4319</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A435">
+        <v>3887</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A436">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A437">
+        <v>5320</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A438">
+        <v>9282</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A439">
+        <v>5857</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A440">
+        <v>6433</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A441">
+        <v>6237</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A442">
+        <v>3723</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A443">
+        <v>7237</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A444">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A445">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A446">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A447">
+        <v>15613</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A448">
+        <v>12512</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A449">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A450">
+        <v>4757</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A451">
+        <v>4076</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A452">
+        <v>5924</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A453">
+        <v>6967</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A454">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A455">
+        <v>4209</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A456">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A457">
+        <v>8071</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A458">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A459">
+        <v>4705</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A460">
+        <v>3962</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A461">
+        <v>4232</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A462">
+        <v>5104</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A463">
+        <v>5524</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A464">
+        <v>5079</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A465">
+        <v>4268</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A466">
+        <v>4066</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A467">
+        <v>5002</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A468">
+        <v>5326</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A469">
+        <v>4222</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A470">
+        <v>5211</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A471">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A472">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A473">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A474">
+        <v>3858</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A475">
+        <v>3293</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A476">
+        <v>3412</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A477">
+        <v>5044</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A478">
+        <v>5397</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A479">
+        <v>5036</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A480">
+        <v>5209</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A481">
+        <v>5220</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A482">
+        <v>8207</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A483">
+        <v>5154</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A484">
+        <v>4816</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A485">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A486">
+        <v>5015</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A487">
+        <v>5181</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A488">
+        <v>5656</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A489">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A490">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A491">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A492">
+        <v>5821</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A493">
+        <v>6076</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A494">
+        <v>8698</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A495">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A496">
+        <v>7151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A65BD1-9673-450E-AE5C-F298837BE8E3}">
+  <dimension ref="A4:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="64.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>95268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>94997</v>
       </c>
     </row>
   </sheetData>
@@ -5463,12 +9268,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E449699B-FFF6-41DB-AE6E-253FE1AB9413}">
-  <dimension ref="B1:E5"/>
+  <dimension ref="B1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5477,61 +9282,70 @@
     <col min="3" max="3" width="57.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="1" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>165</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>600</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>2200</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>5400</v>
+        <v>5800</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>